<commit_message>
Finalized CAD with the EPP foam material integrated
</commit_message>
<xml_diff>
--- a/CAD/naca airfoils.xlsx
+++ b/CAD/naca airfoils.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20357"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\campus\emf\Mech2\dblais6\Desktop\Mech 532 CAD\Airfoil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MECH532\CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8933321-8349-4CF9-93AC-720F96BA0A6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C4268C-784D-4E9B-8282-5E4F60947AD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7590" xr2:uid="{EB129E29-9C87-4BDF-8167-8C5C29152DE1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7590" activeTab="1" xr2:uid="{EB129E29-9C87-4BDF-8167-8C5C29152DE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Wing and Tailplane" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>m</t>
   </si>
@@ -50,18 +51,51 @@
   <si>
     <t>chord_tailplane</t>
   </si>
+  <si>
+    <t>NACA</t>
+  </si>
+  <si>
+    <t>chord length at top</t>
+  </si>
+  <si>
+    <t>chord length at bottom</t>
+  </si>
+  <si>
+    <t>Top part of the fin</t>
+  </si>
+  <si>
+    <t>Bottom part of the fin</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>For cutting plane</t>
+  </si>
+  <si>
+    <t>Cutting plane height in body</t>
+  </si>
+  <si>
+    <t>Offset of cutting plane</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,10 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D548378-1CFF-4BFD-AD04-128A9345765E}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,4 +2141,1658 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2E3A9D-DA5B-4F82-946E-8F4FD58210EA}">
+  <dimension ref="A1:X43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3">
+        <v>0.15</v>
+      </c>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>1.325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1.58E-3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>$N$1*A9</f>
+        <v>0.05</v>
+      </c>
+      <c r="L9">
+        <f>B9*$N$1</f>
+        <v>7.9000000000000009E-5</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>$N$2*A9</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P9">
+        <f>B9*$N$2</f>
+        <v>1.1060000000000002E-4</v>
+      </c>
+      <c r="Q9">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T9">
+        <f>O9+$N$5</f>
+        <v>1.395</v>
+      </c>
+      <c r="U9">
+        <v>1.1060000000000002E-4</v>
+      </c>
+      <c r="V9">
+        <f>$N$4</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="X9">
+        <f>1.33</f>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.95</v>
+      </c>
+      <c r="B10">
+        <v>1.008E-2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>$N$1*A10</f>
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="L10">
+        <f>B10*$N$1</f>
+        <v>5.04E-4</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>$N$2*A10</f>
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="P10">
+        <f>B10*$N$2</f>
+        <v>7.0560000000000013E-4</v>
+      </c>
+      <c r="Q10">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ref="T10:T43" si="0">O10+$N$5</f>
+        <v>1.3915</v>
+      </c>
+      <c r="U10">
+        <v>7.0560000000000013E-4</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ref="V10:V43" si="1">$N$4</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.9</v>
+      </c>
+      <c r="B11">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>$N$1*A11</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="L11">
+        <f>B11*$N$1</f>
+        <v>9.050000000000001E-4</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>$N$2*A11</f>
+        <v>6.3000000000000014E-2</v>
+      </c>
+      <c r="P11">
+        <f>B11*$N$2</f>
+        <v>1.2670000000000003E-3</v>
+      </c>
+      <c r="Q11">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="U11">
+        <v>1.2670000000000003E-3</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.8</v>
+      </c>
+      <c r="B12">
+        <v>3.279E-2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>$N$1*A12</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="L12">
+        <f>B12*$N$1</f>
+        <v>1.6395000000000001E-3</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>$N$2*A12</f>
+        <v>5.6000000000000008E-2</v>
+      </c>
+      <c r="P12">
+        <f>B12*$N$2</f>
+        <v>2.2953000000000001E-3</v>
+      </c>
+      <c r="Q12">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>1.381</v>
+      </c>
+      <c r="U12">
+        <v>2.2953000000000001E-3</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.7</v>
+      </c>
+      <c r="B13">
+        <v>4.58E-2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f>$N$1*A13</f>
+        <v>3.4999999999999996E-2</v>
+      </c>
+      <c r="L13">
+        <f>B13*$N$1</f>
+        <v>2.2899999999999999E-3</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>$N$2*A13</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="P13">
+        <f>B13*$N$2</f>
+        <v>3.2060000000000005E-3</v>
+      </c>
+      <c r="Q13">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>1.3739999999999999</v>
+      </c>
+      <c r="U13">
+        <v>3.2060000000000005E-3</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.6</v>
+      </c>
+      <c r="B14">
+        <v>5.704E-2</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f>$N$1*A14</f>
+        <v>0.03</v>
+      </c>
+      <c r="L14">
+        <f>B14*$N$1</f>
+        <v>2.8520000000000004E-3</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>$N$2*A14</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="P14">
+        <f>B14*$N$2</f>
+        <v>3.9928000000000003E-3</v>
+      </c>
+      <c r="Q14">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>1.367</v>
+      </c>
+      <c r="U14">
+        <v>3.9928000000000003E-3</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.5</v>
+      </c>
+      <c r="B15">
+        <v>6.6170000000000007E-2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>$N$1*A15</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L15">
+        <f>B15*$N$1</f>
+        <v>3.3085000000000007E-3</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>$N$2*A15</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P15">
+        <f>B15*$N$2</f>
+        <v>4.6319000000000013E-3</v>
+      </c>
+      <c r="Q15">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="U15">
+        <v>4.6319000000000013E-3</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.4</v>
+      </c>
+      <c r="B16">
+        <v>7.2539999999999993E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>$N$1*A16</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="L16">
+        <f>B16*$N$1</f>
+        <v>3.627E-3</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>$N$2*A16</f>
+        <v>2.8000000000000004E-2</v>
+      </c>
+      <c r="P16">
+        <f>B16*$N$2</f>
+        <v>5.0778000000000004E-3</v>
+      </c>
+      <c r="Q16">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>1.353</v>
+      </c>
+      <c r="U16">
+        <v>5.0778000000000004E-3</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.3</v>
+      </c>
+      <c r="B17">
+        <v>7.5020000000000003E-2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>$N$1*A17</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L17">
+        <f>B17*$N$1</f>
+        <v>3.7510000000000004E-3</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>$N$2*A17</f>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="P17">
+        <f>B17*$N$2</f>
+        <v>5.2514000000000007E-3</v>
+      </c>
+      <c r="Q17">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>1.3459999999999999</v>
+      </c>
+      <c r="U17">
+        <v>5.2514000000000007E-3</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.25</v>
+      </c>
+      <c r="B18">
+        <v>7.4270000000000003E-2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>$N$1*A18</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="L18">
+        <f>B18*$N$1</f>
+        <v>3.7135000000000002E-3</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>$N$2*A18</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="P18">
+        <f>B18*$N$2</f>
+        <v>5.1989000000000011E-3</v>
+      </c>
+      <c r="Q18">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="0"/>
+        <v>1.3425</v>
+      </c>
+      <c r="U18">
+        <v>5.1989000000000011E-3</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.2</v>
+      </c>
+      <c r="B19">
+        <v>7.1720000000000006E-2</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>$N$1*A19</f>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="L19">
+        <f>B19*$N$1</f>
+        <v>3.5860000000000006E-3</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>$N$2*A19</f>
+        <v>1.4000000000000002E-2</v>
+      </c>
+      <c r="P19">
+        <f>B19*$N$2</f>
+        <v>5.0204000000000013E-3</v>
+      </c>
+      <c r="Q19">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="0"/>
+        <v>1.339</v>
+      </c>
+      <c r="U19">
+        <v>5.0204000000000013E-3</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.15</v>
+      </c>
+      <c r="B20">
+        <v>6.6820000000000004E-2</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>$N$1*A20</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="L20">
+        <f>B20*$N$1</f>
+        <v>3.3410000000000002E-3</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>$N$2*A20</f>
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="P20">
+        <f>B20*$N$2</f>
+        <v>4.6774000000000008E-3</v>
+      </c>
+      <c r="Q20">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="0"/>
+        <v>1.3354999999999999</v>
+      </c>
+      <c r="U20">
+        <v>4.6774000000000008E-3</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.1</v>
+      </c>
+      <c r="B21">
+        <v>5.8529999999999999E-2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>$N$1*A21</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="L21">
+        <f>B21*$N$1</f>
+        <v>2.9265000000000003E-3</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>$N$2*A21</f>
+        <v>7.000000000000001E-3</v>
+      </c>
+      <c r="P21">
+        <f>B21*$N$2</f>
+        <v>4.0971000000000002E-3</v>
+      </c>
+      <c r="Q21">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="0"/>
+        <v>1.3319999999999999</v>
+      </c>
+      <c r="U21">
+        <v>4.0971000000000002E-3</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B22">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>$N$1*A22</f>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="L22">
+        <f>B22*$N$1</f>
+        <v>2.6250000000000002E-3</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>$N$2*A22</f>
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="P22">
+        <f>B22*$N$2</f>
+        <v>3.6750000000000003E-3</v>
+      </c>
+      <c r="Q22">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>1.3302499999999999</v>
+      </c>
+      <c r="U22">
+        <v>3.6750000000000003E-3</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.05</v>
+      </c>
+      <c r="B23">
+        <v>4.4429999999999997E-2</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>$N$1*A23</f>
+        <v>2.5000000000000005E-3</v>
+      </c>
+      <c r="L23">
+        <f>B23*$N$1</f>
+        <v>2.2215E-3</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>$N$2*A23</f>
+        <v>3.5000000000000005E-3</v>
+      </c>
+      <c r="P23">
+        <f>B23*$N$2</f>
+        <v>3.1101000000000002E-3</v>
+      </c>
+      <c r="Q23">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>1.3285</v>
+      </c>
+      <c r="U23">
+        <v>3.1101000000000002E-3</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B24">
+        <v>3.2680000000000001E-2</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>$N$1*A24</f>
+        <v>1.2500000000000002E-3</v>
+      </c>
+      <c r="L24">
+        <f>B24*$N$1</f>
+        <v>1.634E-3</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>$N$2*A24</f>
+        <v>1.7500000000000003E-3</v>
+      </c>
+      <c r="P24">
+        <f>B24*$N$2</f>
+        <v>2.2876000000000003E-3</v>
+      </c>
+      <c r="Q24">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>1.3267499999999999</v>
+      </c>
+      <c r="U24">
+        <v>2.2876000000000003E-3</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="B25">
+        <v>2.367E-2</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>$N$1*A25</f>
+        <v>6.2500000000000012E-4</v>
+      </c>
+      <c r="L25">
+        <f>B25*$N$1</f>
+        <v>1.1835000000000001E-3</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>$N$2*A25</f>
+        <v>8.7500000000000013E-4</v>
+      </c>
+      <c r="P25">
+        <f>B25*$N$2</f>
+        <v>1.6569000000000002E-3</v>
+      </c>
+      <c r="Q25">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>1.3258749999999999</v>
+      </c>
+      <c r="U25">
+        <v>1.6569000000000002E-3</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>$N$1*A26</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>B26*$N$1</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>$N$2*A26</f>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f>B26*$N$2</f>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>1.325</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="B27">
+        <v>-2.367E-2</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>$N$1*A27</f>
+        <v>6.2500000000000012E-4</v>
+      </c>
+      <c r="L27">
+        <f>B27*$N$1</f>
+        <v>-1.1835000000000001E-3</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f>$N$2*A27</f>
+        <v>8.7500000000000013E-4</v>
+      </c>
+      <c r="P27">
+        <f>B27*$N$2</f>
+        <v>-1.6569000000000002E-3</v>
+      </c>
+      <c r="Q27">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>1.3258749999999999</v>
+      </c>
+      <c r="U27">
+        <v>-1.6569000000000002E-3</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B28">
+        <v>-3.2680000000000001E-2</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>$N$1*A28</f>
+        <v>1.2500000000000002E-3</v>
+      </c>
+      <c r="L28">
+        <f>B28*$N$1</f>
+        <v>-1.634E-3</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>$N$2*A28</f>
+        <v>1.7500000000000003E-3</v>
+      </c>
+      <c r="P28">
+        <f>B28*$N$2</f>
+        <v>-2.2876000000000003E-3</v>
+      </c>
+      <c r="Q28">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>1.3267499999999999</v>
+      </c>
+      <c r="U28">
+        <v>-2.2876000000000003E-3</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.05</v>
+      </c>
+      <c r="B29">
+        <v>-4.4429999999999997E-2</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>$N$1*A29</f>
+        <v>2.5000000000000005E-3</v>
+      </c>
+      <c r="L29">
+        <f>B29*$N$1</f>
+        <v>-2.2215E-3</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f>$N$2*A29</f>
+        <v>3.5000000000000005E-3</v>
+      </c>
+      <c r="P29">
+        <f>B29*$N$2</f>
+        <v>-3.1101000000000002E-3</v>
+      </c>
+      <c r="Q29">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>1.3285</v>
+      </c>
+      <c r="U29">
+        <v>-3.1101000000000002E-3</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B30">
+        <v>-5.2499999999999998E-2</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>$N$1*A30</f>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="L30">
+        <f>B30*$N$1</f>
+        <v>-2.6250000000000002E-3</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f>$N$2*A30</f>
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="P30">
+        <f>B30*$N$2</f>
+        <v>-3.6750000000000003E-3</v>
+      </c>
+      <c r="Q30">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>1.3302499999999999</v>
+      </c>
+      <c r="U30">
+        <v>-3.6750000000000003E-3</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.1</v>
+      </c>
+      <c r="B31">
+        <v>-5.8529999999999999E-2</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f>$N$1*A31</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="L31">
+        <f>B31*$N$1</f>
+        <v>-2.9265000000000003E-3</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f>$N$2*A31</f>
+        <v>7.000000000000001E-3</v>
+      </c>
+      <c r="P31">
+        <f>B31*$N$2</f>
+        <v>-4.0971000000000002E-3</v>
+      </c>
+      <c r="Q31">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>1.3319999999999999</v>
+      </c>
+      <c r="U31">
+        <v>-4.0971000000000002E-3</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.15</v>
+      </c>
+      <c r="B32">
+        <v>-6.6820000000000004E-2</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f>$N$1*A32</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="L32">
+        <f>B32*$N$1</f>
+        <v>-3.3410000000000002E-3</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f>$N$2*A32</f>
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="P32">
+        <f>B32*$N$2</f>
+        <v>-4.6774000000000008E-3</v>
+      </c>
+      <c r="Q32">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>1.3354999999999999</v>
+      </c>
+      <c r="U32">
+        <v>-4.6774000000000008E-3</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.2</v>
+      </c>
+      <c r="B33">
+        <v>-7.1720000000000006E-2</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f>$N$1*A33</f>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="L33">
+        <f>B33*$N$1</f>
+        <v>-3.5860000000000006E-3</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f>$N$2*A33</f>
+        <v>1.4000000000000002E-2</v>
+      </c>
+      <c r="P33">
+        <f>B33*$N$2</f>
+        <v>-5.0204000000000013E-3</v>
+      </c>
+      <c r="Q33">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="0"/>
+        <v>1.339</v>
+      </c>
+      <c r="U33">
+        <v>-5.0204000000000013E-3</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.25</v>
+      </c>
+      <c r="B34">
+        <v>-7.4270000000000003E-2</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>$N$1*A34</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="L34">
+        <f>B34*$N$1</f>
+        <v>-3.7135000000000002E-3</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f>$N$2*A34</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="P34">
+        <f>B34*$N$2</f>
+        <v>-5.1989000000000011E-3</v>
+      </c>
+      <c r="Q34">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="0"/>
+        <v>1.3425</v>
+      </c>
+      <c r="U34">
+        <v>-5.1989000000000011E-3</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.3</v>
+      </c>
+      <c r="B35">
+        <v>-7.5020000000000003E-2</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f>$N$1*A35</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L35">
+        <f>B35*$N$1</f>
+        <v>-3.7510000000000004E-3</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f>$N$2*A35</f>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="P35">
+        <f>B35*$N$2</f>
+        <v>-5.2514000000000007E-3</v>
+      </c>
+      <c r="Q35">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="0"/>
+        <v>1.3459999999999999</v>
+      </c>
+      <c r="U35">
+        <v>-5.2514000000000007E-3</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.4</v>
+      </c>
+      <c r="B36">
+        <v>-7.2539999999999993E-2</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f>$N$1*A36</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="L36">
+        <f>B36*$N$1</f>
+        <v>-3.627E-3</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f>$N$2*A36</f>
+        <v>2.8000000000000004E-2</v>
+      </c>
+      <c r="P36">
+        <f>B36*$N$2</f>
+        <v>-5.0778000000000004E-3</v>
+      </c>
+      <c r="Q36">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="0"/>
+        <v>1.353</v>
+      </c>
+      <c r="U36">
+        <v>-5.0778000000000004E-3</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.5</v>
+      </c>
+      <c r="B37">
+        <v>-6.6170000000000007E-2</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f>$N$1*A37</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L37">
+        <f>B37*$N$1</f>
+        <v>-3.3085000000000007E-3</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f>$N$2*A37</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P37">
+        <f>B37*$N$2</f>
+        <v>-4.6319000000000013E-3</v>
+      </c>
+      <c r="Q37">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="0"/>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="U37">
+        <v>-4.6319000000000013E-3</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.6</v>
+      </c>
+      <c r="B38">
+        <v>-5.704E-2</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f>$N$1*A38</f>
+        <v>0.03</v>
+      </c>
+      <c r="L38">
+        <f>B38*$N$1</f>
+        <v>-2.8520000000000004E-3</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f>$N$2*A38</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="P38">
+        <f>B38*$N$2</f>
+        <v>-3.9928000000000003E-3</v>
+      </c>
+      <c r="Q38">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="0"/>
+        <v>1.367</v>
+      </c>
+      <c r="U38">
+        <v>-3.9928000000000003E-3</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.7</v>
+      </c>
+      <c r="B39">
+        <v>-4.58E-2</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f>$N$1*A39</f>
+        <v>3.4999999999999996E-2</v>
+      </c>
+      <c r="L39">
+        <f>B39*$N$1</f>
+        <v>-2.2899999999999999E-3</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f>$N$2*A39</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="P39">
+        <f>B39*$N$2</f>
+        <v>-3.2060000000000005E-3</v>
+      </c>
+      <c r="Q39">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="0"/>
+        <v>1.3739999999999999</v>
+      </c>
+      <c r="U39">
+        <v>-3.2060000000000005E-3</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.8</v>
+      </c>
+      <c r="B40">
+        <v>-3.279E-2</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f>$N$1*A40</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="L40">
+        <f>B40*$N$1</f>
+        <v>-1.6395000000000001E-3</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f>$N$2*A40</f>
+        <v>5.6000000000000008E-2</v>
+      </c>
+      <c r="P40">
+        <f>B40*$N$2</f>
+        <v>-2.2953000000000001E-3</v>
+      </c>
+      <c r="Q40">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="0"/>
+        <v>1.381</v>
+      </c>
+      <c r="U40">
+        <v>-2.2953000000000001E-3</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.9</v>
+      </c>
+      <c r="B41">
+        <v>-1.8100000000000002E-2</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f>$N$1*A41</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="L41">
+        <f>B41*$N$1</f>
+        <v>-9.050000000000001E-4</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f>$N$2*A41</f>
+        <v>6.3000000000000014E-2</v>
+      </c>
+      <c r="P41">
+        <f>B41*$N$2</f>
+        <v>-1.2670000000000003E-3</v>
+      </c>
+      <c r="Q41">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="0"/>
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="U41">
+        <v>-1.2670000000000003E-3</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.95</v>
+      </c>
+      <c r="B42">
+        <v>-1.008E-2</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f>$N$1*A42</f>
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="L42">
+        <f>B42*$N$1</f>
+        <v>-5.04E-4</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f>$N$2*A42</f>
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="P42">
+        <f>B42*$N$2</f>
+        <v>-7.0560000000000013E-4</v>
+      </c>
+      <c r="Q42">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="0"/>
+        <v>1.3915</v>
+      </c>
+      <c r="U42">
+        <v>-7.0560000000000013E-4</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>-1.58E-3</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f>$N$1*A43</f>
+        <v>0.05</v>
+      </c>
+      <c r="L43">
+        <f>B43*$N$1</f>
+        <v>-7.9000000000000009E-5</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <f>$N$2*A43</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P43">
+        <f>B43*$N$2</f>
+        <v>-1.1060000000000002E-4</v>
+      </c>
+      <c r="Q43">
+        <f>$N$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="0"/>
+        <v>1.395</v>
+      </c>
+      <c r="U43">
+        <v>-1.1060000000000002E-4</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>